<commit_message>
3pt and ball control
fixed team ball control stat
rebalanced 3pt shooters
</commit_message>
<xml_diff>
--- a/PlayerInfo.xlsx
+++ b/PlayerInfo.xlsx
@@ -2208,13 +2208,14 @@
   <dimension ref="A1:H493"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C484" sqref="C1:E1048576"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.140625" customWidth="1"/>
     <col min="8" max="8" width="24.7109375" customWidth="1"/>
   </cols>
@@ -2256,7 +2257,7 @@
         <v>495</v>
       </c>
       <c r="H2" t="b">
-        <f>(EXACT(A2,B2))</f>
+        <f t="shared" ref="H2:H65" si="0">(EXACT(A2,B2))</f>
         <v>1</v>
       </c>
     </row>
@@ -2277,7 +2278,7 @@
         <v>552</v>
       </c>
       <c r="H3" t="b">
-        <f>(EXACT(A3,B3))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2298,7 +2299,7 @@
         <v>477</v>
       </c>
       <c r="H4" t="b">
-        <f>(EXACT(A4,B4))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2319,7 +2320,7 @@
         <v>532</v>
       </c>
       <c r="H5" t="b">
-        <f>(EXACT(A5,B5))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2340,7 +2341,7 @@
         <v>503</v>
       </c>
       <c r="H6" t="b">
-        <f>(EXACT(A6,B6))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2361,7 +2362,7 @@
         <v>542</v>
       </c>
       <c r="H7" t="b">
-        <f>(EXACT(A7,B7))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2382,7 +2383,7 @@
         <v>532</v>
       </c>
       <c r="H8" t="b">
-        <f>(EXACT(A8,B8))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2403,7 +2404,7 @@
         <v>493</v>
       </c>
       <c r="H9" t="b">
-        <f>(EXACT(A9,B9))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2424,7 +2425,7 @@
         <v>540</v>
       </c>
       <c r="H10" t="b">
-        <f>(EXACT(A10,B10))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2445,7 +2446,7 @@
         <v>528</v>
       </c>
       <c r="H11" t="b">
-        <f>(EXACT(A11,B11))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2466,7 +2467,7 @@
         <v>542</v>
       </c>
       <c r="H12" t="b">
-        <f>(EXACT(A12,B12))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2487,7 +2488,7 @@
         <v>542</v>
       </c>
       <c r="H13" t="b">
-        <f>(EXACT(A13,B13))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2508,7 +2509,7 @@
         <v>585</v>
       </c>
       <c r="H14" t="b">
-        <f>(EXACT(A14,B14))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2529,7 +2530,7 @@
         <v>487</v>
       </c>
       <c r="H15" t="b">
-        <f>(EXACT(A15,B15))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2550,7 +2551,7 @@
         <v>475</v>
       </c>
       <c r="H16" t="b">
-        <f>(EXACT(A16,B16))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2571,7 +2572,7 @@
         <v>542</v>
       </c>
       <c r="H17" t="b">
-        <f>(EXACT(A17,B17))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2592,7 +2593,7 @@
         <v>542</v>
       </c>
       <c r="H18" t="b">
-        <f>(EXACT(A18,B18))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2613,7 +2614,7 @@
         <v>542</v>
       </c>
       <c r="H19" t="b">
-        <f>(EXACT(A19,B19))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2634,7 +2635,7 @@
         <v>501</v>
       </c>
       <c r="H20" t="b">
-        <f>(EXACT(A20,B20))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2655,7 +2656,7 @@
         <v>495</v>
       </c>
       <c r="H21" t="b">
-        <f>(EXACT(A21,B21))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2676,7 +2677,7 @@
         <v>477</v>
       </c>
       <c r="H22" t="b">
-        <f>(EXACT(A22,B22))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2697,7 +2698,7 @@
         <v>577</v>
       </c>
       <c r="H23" t="b">
-        <f>(EXACT(A23,B23))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2718,7 +2719,7 @@
         <v>493</v>
       </c>
       <c r="H24" t="b">
-        <f>(EXACT(A24,B24))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2739,7 +2740,7 @@
         <v>542</v>
       </c>
       <c r="H25" t="b">
-        <f>(EXACT(A25,B25))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2760,7 +2761,7 @@
         <v>542</v>
       </c>
       <c r="H26" t="b">
-        <f>(EXACT(A26,B26))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2781,7 +2782,7 @@
         <v>577</v>
       </c>
       <c r="H27" t="b">
-        <f>(EXACT(A27,B27))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2802,7 +2803,7 @@
         <v>564</v>
       </c>
       <c r="H28" t="b">
-        <f>(EXACT(A28,B28))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2823,7 +2824,7 @@
         <v>515</v>
       </c>
       <c r="H29" t="b">
-        <f>(EXACT(A29,B29))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2844,7 +2845,7 @@
         <v>539</v>
       </c>
       <c r="H30" t="b">
-        <f>(EXACT(A30,B30))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2865,7 +2866,7 @@
         <v>517</v>
       </c>
       <c r="H31" t="b">
-        <f>(EXACT(A31,B31))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2886,7 +2887,7 @@
         <v>508</v>
       </c>
       <c r="H32" t="b">
-        <f>(EXACT(A32,B32))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2907,7 +2908,7 @@
         <v>496</v>
       </c>
       <c r="H33" t="b">
-        <f>(EXACT(A33,B33))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2928,7 +2929,7 @@
         <v>517</v>
       </c>
       <c r="H34" t="b">
-        <f>(EXACT(A34,B34))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2949,7 +2950,7 @@
         <v>567</v>
       </c>
       <c r="H35" t="b">
-        <f>(EXACT(A35,B35))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2970,7 +2971,7 @@
         <v>587</v>
       </c>
       <c r="H36" t="b">
-        <f>(EXACT(A36,B36))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2991,7 +2992,7 @@
         <v>576</v>
       </c>
       <c r="H37" t="b">
-        <f>(EXACT(A37,B37))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3012,7 +3013,7 @@
         <v>509</v>
       </c>
       <c r="H38" t="b">
-        <f>(EXACT(A38,B38))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3033,7 +3034,7 @@
         <v>501</v>
       </c>
       <c r="H39" t="b">
-        <f>(EXACT(A39,B39))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3054,7 +3055,7 @@
         <v>572</v>
       </c>
       <c r="H40" t="b">
-        <f>(EXACT(A40,B40))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3075,7 +3076,7 @@
         <v>495</v>
       </c>
       <c r="H41" t="b">
-        <f>(EXACT(A41,B41))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3096,7 +3097,7 @@
         <v>515</v>
       </c>
       <c r="H42" t="b">
-        <f>(EXACT(A42,B42))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3117,7 +3118,7 @@
         <v>542</v>
       </c>
       <c r="H43" t="b">
-        <f>(EXACT(A43,B43))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3138,7 +3139,7 @@
         <v>504</v>
       </c>
       <c r="H44" t="b">
-        <f>(EXACT(A44,B44))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3159,7 +3160,7 @@
         <v>542</v>
       </c>
       <c r="H45" t="b">
-        <f>(EXACT(A45,B45))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3180,7 +3181,7 @@
         <v>549</v>
       </c>
       <c r="H46" t="b">
-        <f>(EXACT(A46,B46))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3201,7 +3202,7 @@
         <v>542</v>
       </c>
       <c r="H47" t="b">
-        <f>(EXACT(A47,B47))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3222,7 +3223,7 @@
         <v>542</v>
       </c>
       <c r="H48" t="b">
-        <f>(EXACT(A48,B48))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3243,7 +3244,7 @@
         <v>503</v>
       </c>
       <c r="H49" t="b">
-        <f>(EXACT(A49,B49))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3264,7 +3265,7 @@
         <v>544</v>
       </c>
       <c r="H50" t="b">
-        <f>(EXACT(A50,B50))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3285,7 +3286,7 @@
         <v>522</v>
       </c>
       <c r="H51" t="b">
-        <f>(EXACT(A51,B51))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3306,7 +3307,7 @@
         <v>484</v>
       </c>
       <c r="H52" t="b">
-        <f>(EXACT(A52,B52))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3327,7 +3328,7 @@
         <v>542</v>
       </c>
       <c r="H53" t="b">
-        <f>(EXACT(A53,B53))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3348,7 +3349,7 @@
         <v>517</v>
       </c>
       <c r="H54" t="b">
-        <f>(EXACT(A54,B54))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3369,7 +3370,7 @@
         <v>515</v>
       </c>
       <c r="H55" t="b">
-        <f>(EXACT(A55,B55))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3390,7 +3391,7 @@
         <v>544</v>
       </c>
       <c r="H56" t="b">
-        <f>(EXACT(A56,B56))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3411,7 +3412,7 @@
         <v>498</v>
       </c>
       <c r="H57" t="b">
-        <f>(EXACT(A57,B57))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3432,7 +3433,7 @@
         <v>566</v>
       </c>
       <c r="H58" t="b">
-        <f>(EXACT(A58,B58))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3453,7 +3454,7 @@
         <v>542</v>
       </c>
       <c r="H59" t="b">
-        <f>(EXACT(A59,B59))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3474,7 +3475,7 @@
         <v>555</v>
       </c>
       <c r="H60" t="b">
-        <f>(EXACT(A60,B60))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3495,7 +3496,7 @@
         <v>520</v>
       </c>
       <c r="H61" t="b">
-        <f>(EXACT(A61,B61))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3516,7 +3517,7 @@
         <v>542</v>
       </c>
       <c r="H62" t="b">
-        <f>(EXACT(A62,B62))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3537,7 +3538,7 @@
         <v>569</v>
       </c>
       <c r="H63" t="b">
-        <f>(EXACT(A63,B63))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3558,7 +3559,7 @@
         <v>586</v>
       </c>
       <c r="H64" t="b">
-        <f>(EXACT(A64,B64))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3579,7 +3580,7 @@
         <v>540</v>
       </c>
       <c r="H65" t="b">
-        <f>(EXACT(A65,B65))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3600,7 +3601,7 @@
         <v>556</v>
       </c>
       <c r="H66" t="b">
-        <f>(EXACT(A66,B66))</f>
+        <f t="shared" ref="H66:H129" si="1">(EXACT(A66,B66))</f>
         <v>1</v>
       </c>
     </row>
@@ -3621,7 +3622,7 @@
         <v>501</v>
       </c>
       <c r="H67" t="b">
-        <f>(EXACT(A67,B67))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3642,7 +3643,7 @@
         <v>567</v>
       </c>
       <c r="H68" t="b">
-        <f>(EXACT(A68,B68))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3663,7 +3664,7 @@
         <v>495</v>
       </c>
       <c r="H69" t="b">
-        <f>(EXACT(A69,B69))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3684,7 +3685,7 @@
         <v>516</v>
       </c>
       <c r="H70" t="b">
-        <f>(EXACT(A70,B70))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3705,7 +3706,7 @@
         <v>503</v>
       </c>
       <c r="H71" t="b">
-        <f>(EXACT(A71,B71))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3726,7 +3727,7 @@
         <v>477</v>
       </c>
       <c r="H72" t="b">
-        <f>(EXACT(A72,B72))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3747,7 +3748,7 @@
         <v>495</v>
       </c>
       <c r="H73" t="b">
-        <f>(EXACT(A73,B73))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3768,7 +3769,7 @@
         <v>477</v>
       </c>
       <c r="H74" t="b">
-        <f>(EXACT(A74,B74))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3789,7 +3790,7 @@
         <v>482</v>
       </c>
       <c r="H75" t="b">
-        <f>(EXACT(A75,B75))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3810,7 +3811,7 @@
         <v>508</v>
       </c>
       <c r="H76" t="b">
-        <f>(EXACT(A76,B76))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3831,7 +3832,7 @@
         <v>493</v>
       </c>
       <c r="H77" t="b">
-        <f>(EXACT(A77,B77))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3852,7 +3853,7 @@
         <v>529</v>
       </c>
       <c r="H78" t="b">
-        <f>(EXACT(A78,B78))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3873,7 +3874,7 @@
         <v>498</v>
       </c>
       <c r="H79" t="b">
-        <f>(EXACT(A79,B79))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3894,7 +3895,7 @@
         <v>489</v>
       </c>
       <c r="H80" t="b">
-        <f>(EXACT(A80,B80))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3915,7 +3916,7 @@
         <v>585</v>
       </c>
       <c r="H81" t="b">
-        <f>(EXACT(A81,B81))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3936,7 +3937,7 @@
         <v>517</v>
       </c>
       <c r="H82" t="b">
-        <f>(EXACT(A82,B82))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3957,7 +3958,7 @@
         <v>592</v>
       </c>
       <c r="H83" t="b">
-        <f>(EXACT(A83,B83))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3978,7 +3979,7 @@
         <v>542</v>
       </c>
       <c r="H84" t="b">
-        <f>(EXACT(A84,B84))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3999,7 +4000,7 @@
         <v>512</v>
       </c>
       <c r="H85" t="b">
-        <f>(EXACT(A85,B85))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4020,7 +4021,7 @@
         <v>515</v>
       </c>
       <c r="H86" t="b">
-        <f>(EXACT(A86,B86))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4041,7 +4042,7 @@
         <v>503</v>
       </c>
       <c r="H87" t="b">
-        <f>(EXACT(A87,B87))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4062,7 +4063,7 @@
         <v>480</v>
       </c>
       <c r="H88" t="b">
-        <f>(EXACT(A88,B88))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4083,7 +4084,7 @@
         <v>572</v>
       </c>
       <c r="H89" t="b">
-        <f>(EXACT(A89,B89))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4104,7 +4105,7 @@
         <v>590</v>
       </c>
       <c r="H90" t="b">
-        <f>(EXACT(A90,B90))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4125,7 +4126,7 @@
         <v>572</v>
       </c>
       <c r="H91" t="b">
-        <f>(EXACT(A91,B91))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4146,7 +4147,7 @@
         <v>501</v>
       </c>
       <c r="H92" t="b">
-        <f>(EXACT(A92,B92))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4167,7 +4168,7 @@
         <v>588</v>
       </c>
       <c r="H93" t="b">
-        <f>(EXACT(A93,B93))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4188,7 +4189,7 @@
         <v>542</v>
       </c>
       <c r="H94" t="b">
-        <f>(EXACT(A94,B94))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4209,7 +4210,7 @@
         <v>542</v>
       </c>
       <c r="H95" t="b">
-        <f>(EXACT(A95,B95))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4230,7 +4231,7 @@
         <v>540</v>
       </c>
       <c r="H96" t="b">
-        <f>(EXACT(A96,B96))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4251,7 +4252,7 @@
         <v>544</v>
       </c>
       <c r="H97" t="b">
-        <f>(EXACT(A97,B97))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4272,7 +4273,7 @@
         <v>580</v>
       </c>
       <c r="H98" t="b">
-        <f>(EXACT(A98,B98))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4293,7 +4294,7 @@
         <v>542</v>
       </c>
       <c r="H99" t="b">
-        <f>(EXACT(A99,B99))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4314,7 +4315,7 @@
         <v>517</v>
       </c>
       <c r="H100" t="b">
-        <f>(EXACT(A100,B100))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4335,7 +4336,7 @@
         <v>531</v>
       </c>
       <c r="H101" t="b">
-        <f>(EXACT(A101,B101))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4356,7 +4357,7 @@
         <v>515</v>
       </c>
       <c r="H102" t="b">
-        <f>(EXACT(A102,B102))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4377,7 +4378,7 @@
         <v>576</v>
       </c>
       <c r="H103" t="b">
-        <f>(EXACT(A103,B103))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4398,7 +4399,7 @@
         <v>503</v>
       </c>
       <c r="H104" t="b">
-        <f>(EXACT(A104,B104))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4419,7 +4420,7 @@
         <v>509</v>
       </c>
       <c r="H105" t="b">
-        <f>(EXACT(A105,B105))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4440,7 +4441,7 @@
         <v>576</v>
       </c>
       <c r="H106" t="b">
-        <f>(EXACT(A106,B106))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4461,7 +4462,7 @@
         <v>594</v>
       </c>
       <c r="H107" t="b">
-        <f>(EXACT(A107,B107))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4482,7 +4483,7 @@
         <v>573</v>
       </c>
       <c r="H108" t="b">
-        <f>(EXACT(A108,B108))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4503,7 +4504,7 @@
         <v>554</v>
       </c>
       <c r="H109" t="b">
-        <f>(EXACT(A109,B109))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4524,7 +4525,7 @@
         <v>563</v>
       </c>
       <c r="H110" t="b">
-        <f>(EXACT(A110,B110))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4545,7 +4546,7 @@
         <v>517</v>
       </c>
       <c r="H111" t="b">
-        <f>(EXACT(A111,B111))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4566,7 +4567,7 @@
         <v>534</v>
       </c>
       <c r="H112" t="b">
-        <f>(EXACT(A112,B112))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4587,7 +4588,7 @@
         <v>542</v>
       </c>
       <c r="H113" t="b">
-        <f>(EXACT(A113,B113))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4608,7 +4609,7 @@
         <v>511</v>
       </c>
       <c r="H114" t="b">
-        <f>(EXACT(A114,B114))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4629,7 +4630,7 @@
         <v>508</v>
       </c>
       <c r="H115" t="b">
-        <f>(EXACT(A115,B115))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4650,7 +4651,7 @@
         <v>529</v>
       </c>
       <c r="H116" t="b">
-        <f>(EXACT(A116,B116))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4671,7 +4672,7 @@
         <v>477</v>
       </c>
       <c r="H117" t="b">
-        <f>(EXACT(A117,B117))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4692,7 +4693,7 @@
         <v>593</v>
       </c>
       <c r="H118" t="b">
-        <f>(EXACT(A118,B118))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4713,7 +4714,7 @@
         <v>514</v>
       </c>
       <c r="H119" t="b">
-        <f>(EXACT(A119,B119))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4734,7 +4735,7 @@
         <v>563</v>
       </c>
       <c r="H120" t="b">
-        <f>(EXACT(A120,B120))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4755,7 +4756,7 @@
         <v>567</v>
       </c>
       <c r="H121" t="b">
-        <f>(EXACT(A121,B121))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4776,7 +4777,7 @@
         <v>542</v>
       </c>
       <c r="H122" t="b">
-        <f>(EXACT(A122,B122))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4797,7 +4798,7 @@
         <v>573</v>
       </c>
       <c r="H123" t="b">
-        <f>(EXACT(A123,B123))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4818,7 +4819,7 @@
         <v>542</v>
       </c>
       <c r="H124" t="b">
-        <f>(EXACT(A124,B124))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4839,7 +4840,7 @@
         <v>542</v>
       </c>
       <c r="H125" t="b">
-        <f>(EXACT(A125,B125))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4860,7 +4861,7 @@
         <v>496</v>
       </c>
       <c r="H126" t="b">
-        <f>(EXACT(A126,B126))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4881,7 +4882,7 @@
         <v>532</v>
       </c>
       <c r="H127" t="b">
-        <f>(EXACT(A127,B127))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4902,7 +4903,7 @@
         <v>515</v>
       </c>
       <c r="H128" t="b">
-        <f>(EXACT(A128,B128))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4923,7 +4924,7 @@
         <v>540</v>
       </c>
       <c r="H129" t="b">
-        <f>(EXACT(A129,B129))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4944,7 +4945,7 @@
         <v>526</v>
       </c>
       <c r="H130" t="b">
-        <f>(EXACT(A130,B130))</f>
+        <f t="shared" ref="H130:H193" si="2">(EXACT(A130,B130))</f>
         <v>1</v>
       </c>
     </row>
@@ -4965,7 +4966,7 @@
         <v>542</v>
       </c>
       <c r="H131" t="b">
-        <f>(EXACT(A131,B131))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -4986,7 +4987,7 @@
         <v>566</v>
       </c>
       <c r="H132" t="b">
-        <f>(EXACT(A132,B132))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5007,7 +5008,7 @@
         <v>526</v>
       </c>
       <c r="H133" t="b">
-        <f>(EXACT(A133,B133))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5028,7 +5029,7 @@
         <v>529</v>
       </c>
       <c r="H134" t="b">
-        <f>(EXACT(A134,B134))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5049,7 +5050,7 @@
         <v>525</v>
       </c>
       <c r="H135" t="b">
-        <f>(EXACT(A135,B135))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5070,7 +5071,7 @@
         <v>544</v>
       </c>
       <c r="H136" t="b">
-        <f>(EXACT(A136,B136))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5091,7 +5092,7 @@
         <v>480</v>
       </c>
       <c r="H137" t="b">
-        <f>(EXACT(A137,B137))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5112,7 +5113,7 @@
         <v>524</v>
       </c>
       <c r="H138" t="b">
-        <f>(EXACT(A138,B138))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5133,7 +5134,7 @@
         <v>476</v>
       </c>
       <c r="H139" t="b">
-        <f>(EXACT(A139,B139))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5154,7 +5155,7 @@
         <v>529</v>
       </c>
       <c r="H140" t="b">
-        <f>(EXACT(A140,B140))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5175,7 +5176,7 @@
         <v>501</v>
       </c>
       <c r="H141" t="b">
-        <f>(EXACT(A141,B141))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5196,7 +5197,7 @@
         <v>517</v>
       </c>
       <c r="H142" t="b">
-        <f>(EXACT(A142,B142))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5217,7 +5218,7 @@
         <v>517</v>
       </c>
       <c r="H143" t="b">
-        <f>(EXACT(A143,B143))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5238,7 +5239,7 @@
         <v>512</v>
       </c>
       <c r="H144" t="b">
-        <f>(EXACT(A144,B144))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5259,7 +5260,7 @@
         <v>553</v>
       </c>
       <c r="H145" t="b">
-        <f>(EXACT(A145,B145))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5280,7 +5281,7 @@
         <v>584</v>
       </c>
       <c r="H146" t="b">
-        <f>(EXACT(A146,B146))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5301,7 +5302,7 @@
         <v>542</v>
       </c>
       <c r="H147" t="b">
-        <f>(EXACT(A147,B147))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5322,7 +5323,7 @@
         <v>556</v>
       </c>
       <c r="H148" t="b">
-        <f>(EXACT(A148,B148))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5343,7 +5344,7 @@
         <v>542</v>
       </c>
       <c r="H149" t="b">
-        <f>(EXACT(A149,B149))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5364,7 +5365,7 @@
         <v>548</v>
       </c>
       <c r="H150" t="b">
-        <f>(EXACT(A150,B150))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5385,7 +5386,7 @@
         <v>579</v>
       </c>
       <c r="H151" t="b">
-        <f>(EXACT(A151,B151))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5406,7 +5407,7 @@
         <v>525</v>
       </c>
       <c r="H152" t="b">
-        <f>(EXACT(A152,B152))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5427,7 +5428,7 @@
         <v>542</v>
       </c>
       <c r="H153" t="b">
-        <f>(EXACT(A153,B153))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5448,7 +5449,7 @@
         <v>592</v>
       </c>
       <c r="H154" t="b">
-        <f>(EXACT(A154,B154))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5469,7 +5470,7 @@
         <v>522</v>
       </c>
       <c r="H155" t="b">
-        <f>(EXACT(A155,B155))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5490,7 +5491,7 @@
         <v>532</v>
       </c>
       <c r="H156" t="b">
-        <f>(EXACT(A156,B156))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5511,7 +5512,7 @@
         <v>574</v>
       </c>
       <c r="H157" t="b">
-        <f>(EXACT(A157,B157))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5532,7 +5533,7 @@
         <v>513</v>
       </c>
       <c r="H158" t="b">
-        <f>(EXACT(A158,B158))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5553,7 +5554,7 @@
         <v>542</v>
       </c>
       <c r="H159" t="b">
-        <f>(EXACT(A159,B159))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5574,7 +5575,7 @@
         <v>501</v>
       </c>
       <c r="H160" t="b">
-        <f>(EXACT(A160,B160))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5595,7 +5596,7 @@
         <v>475</v>
       </c>
       <c r="H161" t="b">
-        <f>(EXACT(A161,B161))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5616,7 +5617,7 @@
         <v>542</v>
       </c>
       <c r="H162" t="b">
-        <f>(EXACT(A162,B162))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5637,7 +5638,7 @@
         <v>522</v>
       </c>
       <c r="H163" t="b">
-        <f>(EXACT(A163,B163))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5658,7 +5659,7 @@
         <v>508</v>
       </c>
       <c r="H164" t="b">
-        <f>(EXACT(A164,B164))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5679,7 +5680,7 @@
         <v>531</v>
       </c>
       <c r="H165" t="b">
-        <f>(EXACT(A165,B165))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5700,7 +5701,7 @@
         <v>542</v>
       </c>
       <c r="H166" t="b">
-        <f>(EXACT(A166,B166))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5721,7 +5722,7 @@
         <v>486</v>
       </c>
       <c r="H167" t="b">
-        <f>(EXACT(A167,B167))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5742,7 +5743,7 @@
         <v>525</v>
       </c>
       <c r="H168" t="b">
-        <f>(EXACT(A168,B168))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5763,7 +5764,7 @@
         <v>477</v>
       </c>
       <c r="H169" t="b">
-        <f>(EXACT(A169,B169))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5784,7 +5785,7 @@
         <v>506</v>
       </c>
       <c r="H170" t="b">
-        <f>(EXACT(A170,B170))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5805,7 +5806,7 @@
         <v>505</v>
       </c>
       <c r="H171" t="b">
-        <f>(EXACT(A171,B171))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5826,7 +5827,7 @@
         <v>593</v>
       </c>
       <c r="H172" t="b">
-        <f>(EXACT(A172,B172))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5847,7 +5848,7 @@
         <v>528</v>
       </c>
       <c r="H173" t="b">
-        <f>(EXACT(A173,B173))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5868,7 +5869,7 @@
         <v>544</v>
       </c>
       <c r="H174" t="b">
-        <f>(EXACT(A174,B174))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5889,7 +5890,7 @@
         <v>527</v>
       </c>
       <c r="H175" t="b">
-        <f>(EXACT(A175,B175))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5910,7 +5911,7 @@
         <v>542</v>
       </c>
       <c r="H176" t="b">
-        <f>(EXACT(A176,B176))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5931,7 +5932,7 @@
         <v>506</v>
       </c>
       <c r="H177" t="b">
-        <f>(EXACT(A177,B177))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5952,7 +5953,7 @@
         <v>516</v>
       </c>
       <c r="H178" t="b">
-        <f>(EXACT(A178,B178))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5973,7 +5974,7 @@
         <v>506</v>
       </c>
       <c r="H179" t="b">
-        <f>(EXACT(A179,B179))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5994,7 +5995,7 @@
         <v>481</v>
       </c>
       <c r="H180" t="b">
-        <f>(EXACT(A180,B180))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -6015,7 +6016,7 @@
         <v>542</v>
       </c>
       <c r="H181" t="b">
-        <f>(EXACT(A181,B181))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -6036,7 +6037,7 @@
         <v>508</v>
       </c>
       <c r="H182" t="b">
-        <f>(EXACT(A182,B182))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -6057,7 +6058,7 @@
         <v>537</v>
       </c>
       <c r="H183" t="b">
-        <f>(EXACT(A183,B183))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -6078,7 +6079,7 @@
         <v>586</v>
       </c>
       <c r="H184" t="b">
-        <f>(EXACT(A184,B184))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -6099,7 +6100,7 @@
         <v>585</v>
       </c>
       <c r="H185" t="b">
-        <f>(EXACT(A185,B185))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -6120,7 +6121,7 @@
         <v>545</v>
       </c>
       <c r="H186" t="b">
-        <f>(EXACT(A186,B186))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -6141,7 +6142,7 @@
         <v>501</v>
       </c>
       <c r="H187" t="b">
-        <f>(EXACT(A187,B187))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -6162,7 +6163,7 @@
         <v>542</v>
       </c>
       <c r="H188" t="b">
-        <f>(EXACT(A188,B188))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -6183,7 +6184,7 @@
         <v>534</v>
       </c>
       <c r="H189" t="b">
-        <f>(EXACT(A189,B189))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -6204,7 +6205,7 @@
         <v>501</v>
       </c>
       <c r="H190" t="b">
-        <f>(EXACT(A190,B190))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -6225,7 +6226,7 @@
         <v>547</v>
       </c>
       <c r="H191" t="b">
-        <f>(EXACT(A191,B191))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -6246,7 +6247,7 @@
         <v>526</v>
       </c>
       <c r="H192" t="b">
-        <f>(EXACT(A192,B192))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -6267,7 +6268,7 @@
         <v>565</v>
       </c>
       <c r="H193" t="b">
-        <f>(EXACT(A193,B193))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -6288,7 +6289,7 @@
         <v>560</v>
       </c>
       <c r="H194" t="b">
-        <f>(EXACT(A194,B194))</f>
+        <f t="shared" ref="H194:H257" si="3">(EXACT(A194,B194))</f>
         <v>1</v>
       </c>
     </row>
@@ -6309,7 +6310,7 @@
         <v>531</v>
       </c>
       <c r="H195" t="b">
-        <f>(EXACT(A195,B195))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6330,7 +6331,7 @@
         <v>558</v>
       </c>
       <c r="H196" t="b">
-        <f>(EXACT(A196,B196))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6351,7 +6352,7 @@
         <v>521</v>
       </c>
       <c r="H197" t="b">
-        <f>(EXACT(A197,B197))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6372,7 +6373,7 @@
         <v>478</v>
       </c>
       <c r="H198" t="b">
-        <f>(EXACT(A198,B198))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6393,7 +6394,7 @@
         <v>585</v>
       </c>
       <c r="H199" t="b">
-        <f>(EXACT(A199,B199))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6414,7 +6415,7 @@
         <v>530</v>
       </c>
       <c r="H200" t="b">
-        <f>(EXACT(A200,B200))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6435,7 +6436,7 @@
         <v>544</v>
       </c>
       <c r="H201" t="b">
-        <f>(EXACT(A201,B201))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6456,7 +6457,7 @@
         <v>517</v>
       </c>
       <c r="H202" t="b">
-        <f>(EXACT(A202,B202))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6477,7 +6478,7 @@
         <v>475</v>
       </c>
       <c r="H203" t="b">
-        <f>(EXACT(A203,B203))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6498,7 +6499,7 @@
         <v>479</v>
       </c>
       <c r="H204" t="b">
-        <f>(EXACT(A204,B204))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6519,7 +6520,7 @@
         <v>553</v>
       </c>
       <c r="H205" t="b">
-        <f>(EXACT(A205,B205))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6540,7 +6541,7 @@
         <v>483</v>
       </c>
       <c r="H206" t="b">
-        <f>(EXACT(A206,B206))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6561,7 +6562,7 @@
         <v>548</v>
       </c>
       <c r="H207" t="b">
-        <f>(EXACT(A207,B207))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6582,7 +6583,7 @@
         <v>569</v>
       </c>
       <c r="H208" t="b">
-        <f>(EXACT(A208,B208))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6603,7 +6604,7 @@
         <v>508</v>
       </c>
       <c r="H209" t="b">
-        <f>(EXACT(A209,B209))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6624,7 +6625,7 @@
         <v>490</v>
       </c>
       <c r="H210" t="b">
-        <f>(EXACT(A210,B210))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6645,7 +6646,7 @@
         <v>532</v>
       </c>
       <c r="H211" t="b">
-        <f>(EXACT(A211,B211))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6666,7 +6667,7 @@
         <v>494</v>
       </c>
       <c r="H212" t="b">
-        <f>(EXACT(A212,B212))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6687,7 +6688,7 @@
         <v>477</v>
       </c>
       <c r="H213" t="b">
-        <f>(EXACT(A213,B213))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6708,7 +6709,7 @@
         <v>557</v>
       </c>
       <c r="H214" t="b">
-        <f>(EXACT(A214,B214))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6729,7 +6730,7 @@
         <v>538</v>
       </c>
       <c r="H215" t="b">
-        <f>(EXACT(A215,B215))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6750,7 +6751,7 @@
         <v>495</v>
       </c>
       <c r="H216" t="b">
-        <f>(EXACT(A216,B216))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6771,7 +6772,7 @@
         <v>478</v>
       </c>
       <c r="H217" t="b">
-        <f>(EXACT(A217,B217))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6792,7 +6793,7 @@
         <v>506</v>
       </c>
       <c r="H218" t="b">
-        <f>(EXACT(A218,B218))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6813,7 +6814,7 @@
         <v>585</v>
       </c>
       <c r="H219" t="b">
-        <f>(EXACT(A219,B219))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6834,7 +6835,7 @@
         <v>515</v>
       </c>
       <c r="H220" t="b">
-        <f>(EXACT(A220,B220))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6855,7 +6856,7 @@
         <v>579</v>
       </c>
       <c r="H221" t="b">
-        <f>(EXACT(A221,B221))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6876,7 +6877,7 @@
         <v>567</v>
       </c>
       <c r="H222" t="b">
-        <f>(EXACT(A222,B222))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6897,7 +6898,7 @@
         <v>526</v>
       </c>
       <c r="H223" t="b">
-        <f>(EXACT(A223,B223))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6918,7 +6919,7 @@
         <v>590</v>
       </c>
       <c r="H224" t="b">
-        <f>(EXACT(A224,B224))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6939,7 +6940,7 @@
         <v>495</v>
       </c>
       <c r="H225" t="b">
-        <f>(EXACT(A225,B225))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6960,7 +6961,7 @@
         <v>510</v>
       </c>
       <c r="H226" t="b">
-        <f>(EXACT(A226,B226))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6981,7 +6982,7 @@
         <v>575</v>
       </c>
       <c r="H227" t="b">
-        <f>(EXACT(A227,B227))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7002,7 +7003,7 @@
         <v>542</v>
       </c>
       <c r="H228" t="b">
-        <f>(EXACT(A228,B228))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7023,7 +7024,7 @@
         <v>477</v>
       </c>
       <c r="H229" t="b">
-        <f>(EXACT(A229,B229))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7044,7 +7045,7 @@
         <v>484</v>
       </c>
       <c r="H230" t="b">
-        <f>(EXACT(A230,B230))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7065,7 +7066,7 @@
         <v>526</v>
       </c>
       <c r="H231" t="b">
-        <f>(EXACT(A231,B231))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7086,7 +7087,7 @@
         <v>503</v>
       </c>
       <c r="H232" t="b">
-        <f>(EXACT(A232,B232))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7107,7 +7108,7 @@
         <v>517</v>
       </c>
       <c r="H233" t="b">
-        <f>(EXACT(A233,B233))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7128,7 +7129,7 @@
         <v>581</v>
       </c>
       <c r="H234" t="b">
-        <f>(EXACT(A234,B234))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7149,7 +7150,7 @@
         <v>542</v>
       </c>
       <c r="H235" t="b">
-        <f>(EXACT(A235,B235))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7170,7 +7171,7 @@
         <v>479</v>
       </c>
       <c r="H236" t="b">
-        <f>(EXACT(A236,B236))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7191,7 +7192,7 @@
         <v>539</v>
       </c>
       <c r="H237" t="b">
-        <f>(EXACT(A237,B237))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7212,7 +7213,7 @@
         <v>542</v>
       </c>
       <c r="H238" t="b">
-        <f>(EXACT(A238,B238))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7233,7 +7234,7 @@
         <v>529</v>
       </c>
       <c r="H239" t="b">
-        <f>(EXACT(A239,B239))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7254,7 +7255,7 @@
         <v>542</v>
       </c>
       <c r="H240" t="b">
-        <f>(EXACT(A240,B240))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7275,7 +7276,7 @@
         <v>544</v>
       </c>
       <c r="H241" t="b">
-        <f>(EXACT(A241,B241))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7296,7 +7297,7 @@
         <v>579</v>
       </c>
       <c r="H242" t="b">
-        <f>(EXACT(A242,B242))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7317,7 +7318,7 @@
         <v>550</v>
       </c>
       <c r="H243" t="b">
-        <f>(EXACT(A243,B243))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7338,7 +7339,7 @@
         <v>530</v>
       </c>
       <c r="H244" t="b">
-        <f>(EXACT(A244,B244))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7359,7 +7360,7 @@
         <v>517</v>
       </c>
       <c r="H245" t="b">
-        <f>(EXACT(A245,B245))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7380,7 +7381,7 @@
         <v>522</v>
       </c>
       <c r="H246" t="b">
-        <f>(EXACT(A246,B246))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7401,7 +7402,7 @@
         <v>593</v>
       </c>
       <c r="H247" t="b">
-        <f>(EXACT(A247,B247))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7422,7 +7423,7 @@
         <v>542</v>
       </c>
       <c r="H248" t="b">
-        <f>(EXACT(A248,B248))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7443,7 +7444,7 @@
         <v>542</v>
       </c>
       <c r="H249" t="b">
-        <f>(EXACT(A249,B249))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7464,7 +7465,7 @@
         <v>576</v>
       </c>
       <c r="H250" t="b">
-        <f>(EXACT(A250,B250))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7485,7 +7486,7 @@
         <v>534</v>
       </c>
       <c r="H251" t="b">
-        <f>(EXACT(A251,B251))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7506,7 +7507,7 @@
         <v>576</v>
       </c>
       <c r="H252" t="b">
-        <f>(EXACT(A252,B252))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7527,7 +7528,7 @@
         <v>572</v>
       </c>
       <c r="H253" t="b">
-        <f>(EXACT(A253,B253))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7548,7 +7549,7 @@
         <v>477</v>
       </c>
       <c r="H254" t="b">
-        <f>(EXACT(A254,B254))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7569,7 +7570,7 @@
         <v>488</v>
       </c>
       <c r="H255" t="b">
-        <f>(EXACT(A255,B255))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7590,7 +7591,7 @@
         <v>546</v>
       </c>
       <c r="H256" t="b">
-        <f>(EXACT(A256,B256))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7611,7 +7612,7 @@
         <v>542</v>
       </c>
       <c r="H257" t="b">
-        <f>(EXACT(A257,B257))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -7632,7 +7633,7 @@
         <v>501</v>
       </c>
       <c r="H258" t="b">
-        <f>(EXACT(A258,B258))</f>
+        <f t="shared" ref="H258:H321" si="4">(EXACT(A258,B258))</f>
         <v>1</v>
       </c>
     </row>
@@ -7653,7 +7654,7 @@
         <v>542</v>
       </c>
       <c r="H259" t="b">
-        <f>(EXACT(A259,B259))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -7674,7 +7675,7 @@
         <v>576</v>
       </c>
       <c r="H260" t="b">
-        <f>(EXACT(A260,B260))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -7695,7 +7696,7 @@
         <v>517</v>
       </c>
       <c r="H261" t="b">
-        <f>(EXACT(A261,B261))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -7716,7 +7717,7 @@
         <v>522</v>
       </c>
       <c r="H262" t="b">
-        <f>(EXACT(A262,B262))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -7737,7 +7738,7 @@
         <v>586</v>
       </c>
       <c r="H263" t="b">
-        <f>(EXACT(A263,B263))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -7758,7 +7759,7 @@
         <v>542</v>
       </c>
       <c r="H264" t="b">
-        <f>(EXACT(A264,B264))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -7779,7 +7780,7 @@
         <v>491</v>
       </c>
       <c r="H265" t="b">
-        <f>(EXACT(A265,B265))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -7800,7 +7801,7 @@
         <v>532</v>
       </c>
       <c r="H266" t="b">
-        <f>(EXACT(A266,B266))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -7821,7 +7822,7 @@
         <v>560</v>
       </c>
       <c r="H267" t="b">
-        <f>(EXACT(A267,B267))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -7842,7 +7843,7 @@
         <v>509</v>
       </c>
       <c r="H268" t="b">
-        <f>(EXACT(A268,B268))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -7863,7 +7864,7 @@
         <v>495</v>
       </c>
       <c r="H269" t="b">
-        <f>(EXACT(A269,B269))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -7884,7 +7885,7 @@
         <v>544</v>
       </c>
       <c r="H270" t="b">
-        <f>(EXACT(A270,B270))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -7905,7 +7906,7 @@
         <v>542</v>
       </c>
       <c r="H271" t="b">
-        <f>(EXACT(A271,B271))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -7926,7 +7927,7 @@
         <v>536</v>
       </c>
       <c r="H272" t="b">
-        <f>(EXACT(A272,B272))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -7947,7 +7948,7 @@
         <v>551</v>
       </c>
       <c r="H273" t="b">
-        <f>(EXACT(A273,B273))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -7968,7 +7969,7 @@
         <v>507</v>
       </c>
       <c r="H274" t="b">
-        <f>(EXACT(A274,B274))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -7989,7 +7990,7 @@
         <v>490</v>
       </c>
       <c r="H275" t="b">
-        <f>(EXACT(A275,B275))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8010,7 +8011,7 @@
         <v>572</v>
       </c>
       <c r="H276" t="b">
-        <f>(EXACT(A276,B276))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8031,7 +8032,7 @@
         <v>542</v>
       </c>
       <c r="H277" t="b">
-        <f>(EXACT(A277,B277))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8052,7 +8053,7 @@
         <v>576</v>
       </c>
       <c r="H278" t="b">
-        <f>(EXACT(A278,B278))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8073,7 +8074,7 @@
         <v>589</v>
       </c>
       <c r="H279" t="b">
-        <f>(EXACT(A279,B279))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8094,7 +8095,7 @@
         <v>519</v>
       </c>
       <c r="H280" t="b">
-        <f>(EXACT(A280,B280))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8115,7 +8116,7 @@
         <v>573</v>
       </c>
       <c r="H281" t="b">
-        <f>(EXACT(A281,B281))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8136,7 +8137,7 @@
         <v>515</v>
       </c>
       <c r="H282" t="b">
-        <f>(EXACT(A282,B282))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8157,7 +8158,7 @@
         <v>587</v>
       </c>
       <c r="H283" t="b">
-        <f>(EXACT(A283,B283))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8178,7 +8179,7 @@
         <v>542</v>
       </c>
       <c r="H284" t="b">
-        <f>(EXACT(A284,B284))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8199,7 +8200,7 @@
         <v>548</v>
       </c>
       <c r="H285" t="b">
-        <f>(EXACT(A285,B285))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8220,7 +8221,7 @@
         <v>542</v>
       </c>
       <c r="H286" t="b">
-        <f>(EXACT(A286,B286))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8241,7 +8242,7 @@
         <v>533</v>
       </c>
       <c r="H287" t="b">
-        <f>(EXACT(A287,B287))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8262,7 +8263,7 @@
         <v>576</v>
       </c>
       <c r="H288" t="b">
-        <f>(EXACT(A288,B288))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8283,7 +8284,7 @@
         <v>496</v>
       </c>
       <c r="H289" t="b">
-        <f>(EXACT(A289,B289))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8304,7 +8305,7 @@
         <v>580</v>
       </c>
       <c r="H290" t="b">
-        <f>(EXACT(A290,B290))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8325,7 +8326,7 @@
         <v>543</v>
       </c>
       <c r="H291" t="b">
-        <f>(EXACT(A291,B291))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8346,7 +8347,7 @@
         <v>501</v>
       </c>
       <c r="H292" t="b">
-        <f>(EXACT(A292,B292))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8367,7 +8368,7 @@
         <v>501</v>
       </c>
       <c r="H293" t="b">
-        <f>(EXACT(A293,B293))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8388,7 +8389,7 @@
         <v>572</v>
       </c>
       <c r="H294" t="b">
-        <f>(EXACT(A294,B294))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8409,7 +8410,7 @@
         <v>490</v>
       </c>
       <c r="H295" t="b">
-        <f>(EXACT(A295,B295))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8430,7 +8431,7 @@
         <v>501</v>
       </c>
       <c r="H296" t="b">
-        <f>(EXACT(A296,B296))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8451,7 +8452,7 @@
         <v>566</v>
       </c>
       <c r="H297" t="b">
-        <f>(EXACT(A297,B297))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8472,7 +8473,7 @@
         <v>558</v>
       </c>
       <c r="H298" t="b">
-        <f>(EXACT(A298,B298))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8493,7 +8494,7 @@
         <v>576</v>
       </c>
       <c r="H299" t="b">
-        <f>(EXACT(A299,B299))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8514,7 +8515,7 @@
         <v>582</v>
       </c>
       <c r="H300" t="b">
-        <f>(EXACT(A300,B300))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8535,7 +8536,7 @@
         <v>568</v>
       </c>
       <c r="H301" t="b">
-        <f>(EXACT(A301,B301))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8556,7 +8557,7 @@
         <v>542</v>
       </c>
       <c r="H302" t="b">
-        <f>(EXACT(A302,B302))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8577,7 +8578,7 @@
         <v>542</v>
       </c>
       <c r="H303" t="b">
-        <f>(EXACT(A303,B303))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8598,7 +8599,7 @@
         <v>571</v>
       </c>
       <c r="H304" t="b">
-        <f>(EXACT(A304,B304))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8619,7 +8620,7 @@
         <v>545</v>
       </c>
       <c r="H305" t="b">
-        <f>(EXACT(A305,B305))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8640,7 +8641,7 @@
         <v>542</v>
       </c>
       <c r="H306" t="b">
-        <f>(EXACT(A306,B306))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8661,7 +8662,7 @@
         <v>539</v>
       </c>
       <c r="H307" t="b">
-        <f>(EXACT(A307,B307))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8682,7 +8683,7 @@
         <v>576</v>
       </c>
       <c r="H308" t="b">
-        <f>(EXACT(A308,B308))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8703,7 +8704,7 @@
         <v>542</v>
       </c>
       <c r="H309" t="b">
-        <f>(EXACT(A309,B309))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8724,7 +8725,7 @@
         <v>542</v>
       </c>
       <c r="H310" t="b">
-        <f>(EXACT(A310,B310))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8745,7 +8746,7 @@
         <v>542</v>
       </c>
       <c r="H311" t="b">
-        <f>(EXACT(A311,B311))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8766,7 +8767,7 @@
         <v>538</v>
       </c>
       <c r="H312" t="b">
-        <f>(EXACT(A312,B312))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8787,7 +8788,7 @@
         <v>552</v>
       </c>
       <c r="H313" t="b">
-        <f>(EXACT(A313,B313))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8808,7 +8809,7 @@
         <v>501</v>
       </c>
       <c r="H314" t="b">
-        <f>(EXACT(A314,B314))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8829,7 +8830,7 @@
         <v>576</v>
       </c>
       <c r="H315" t="b">
-        <f>(EXACT(A315,B315))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8850,7 +8851,7 @@
         <v>560</v>
       </c>
       <c r="H316" t="b">
-        <f>(EXACT(A316,B316))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8871,7 +8872,7 @@
         <v>542</v>
       </c>
       <c r="H317" t="b">
-        <f>(EXACT(A317,B317))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8892,7 +8893,7 @@
         <v>542</v>
       </c>
       <c r="H318" t="b">
-        <f>(EXACT(A318,B318))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8913,7 +8914,7 @@
         <v>542</v>
       </c>
       <c r="H319" t="b">
-        <f>(EXACT(A319,B319))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8934,7 +8935,7 @@
         <v>542</v>
       </c>
       <c r="H320" t="b">
-        <f>(EXACT(A320,B320))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8955,7 +8956,7 @@
         <v>515</v>
       </c>
       <c r="H321" t="b">
-        <f>(EXACT(A321,B321))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -8976,7 +8977,7 @@
         <v>550</v>
       </c>
       <c r="H322" t="b">
-        <f>(EXACT(A322,B322))</f>
+        <f t="shared" ref="H322:H385" si="5">(EXACT(A322,B322))</f>
         <v>1</v>
       </c>
     </row>
@@ -8997,7 +8998,7 @@
         <v>522</v>
       </c>
       <c r="H323" t="b">
-        <f>(EXACT(A323,B323))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9018,7 +9019,7 @@
         <v>515</v>
       </c>
       <c r="H324" t="b">
-        <f>(EXACT(A324,B324))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9039,7 +9040,7 @@
         <v>550</v>
       </c>
       <c r="H325" t="b">
-        <f>(EXACT(A325,B325))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9060,7 +9061,7 @@
         <v>515</v>
       </c>
       <c r="H326" t="b">
-        <f>(EXACT(A326,B326))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9081,7 +9082,7 @@
         <v>503</v>
       </c>
       <c r="H327" t="b">
-        <f>(EXACT(A327,B327))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9102,7 +9103,7 @@
         <v>542</v>
       </c>
       <c r="H328" t="b">
-        <f>(EXACT(A328,B328))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9123,7 +9124,7 @@
         <v>544</v>
       </c>
       <c r="H329" t="b">
-        <f>(EXACT(A329,B329))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9144,7 +9145,7 @@
         <v>501</v>
       </c>
       <c r="H330" t="b">
-        <f>(EXACT(A330,B330))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9165,7 +9166,7 @@
         <v>576</v>
       </c>
       <c r="H331" t="b">
-        <f>(EXACT(A331,B331))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9186,7 +9187,7 @@
         <v>503</v>
       </c>
       <c r="H332" t="b">
-        <f>(EXACT(A332,B332))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9207,7 +9208,7 @@
         <v>559</v>
       </c>
       <c r="H333" t="b">
-        <f>(EXACT(A333,B333))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9228,7 +9229,7 @@
         <v>565</v>
       </c>
       <c r="H334" t="b">
-        <f>(EXACT(A334,B334))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9249,7 +9250,7 @@
         <v>511</v>
       </c>
       <c r="H335" t="b">
-        <f>(EXACT(A335,B335))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9270,7 +9271,7 @@
         <v>516</v>
       </c>
       <c r="H336" t="b">
-        <f>(EXACT(A336,B336))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9291,7 +9292,7 @@
         <v>567</v>
       </c>
       <c r="H337" t="b">
-        <f>(EXACT(A337,B337))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9312,7 +9313,7 @@
         <v>517</v>
       </c>
       <c r="H338" t="b">
-        <f>(EXACT(A338,B338))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9333,7 +9334,7 @@
         <v>548</v>
       </c>
       <c r="H339" t="b">
-        <f>(EXACT(A339,B339))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9354,7 +9355,7 @@
         <v>501</v>
       </c>
       <c r="H340" t="b">
-        <f>(EXACT(A340,B340))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9375,7 +9376,7 @@
         <v>503</v>
       </c>
       <c r="H341" t="b">
-        <f>(EXACT(A341,B341))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9396,7 +9397,7 @@
         <v>485</v>
       </c>
       <c r="H342" t="b">
-        <f>(EXACT(A342,B342))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9417,7 +9418,7 @@
         <v>581</v>
       </c>
       <c r="H343" t="b">
-        <f>(EXACT(A343,B343))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9438,7 +9439,7 @@
         <v>501</v>
       </c>
       <c r="H344" t="b">
-        <f>(EXACT(A344,B344))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9459,7 +9460,7 @@
         <v>542</v>
       </c>
       <c r="H345" t="b">
-        <f>(EXACT(A345,B345))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9480,7 +9481,7 @@
         <v>542</v>
       </c>
       <c r="H346" t="b">
-        <f>(EXACT(A346,B346))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9501,7 +9502,7 @@
         <v>531</v>
       </c>
       <c r="H347" t="b">
-        <f>(EXACT(A347,B347))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9522,7 +9523,7 @@
         <v>475</v>
       </c>
       <c r="H348" t="b">
-        <f>(EXACT(A348,B348))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9543,7 +9544,7 @@
         <v>542</v>
       </c>
       <c r="H349" t="b">
-        <f>(EXACT(A349,B349))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9564,7 +9565,7 @@
         <v>586</v>
       </c>
       <c r="H350" t="b">
-        <f>(EXACT(A350,B350))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9585,7 +9586,7 @@
         <v>562</v>
       </c>
       <c r="H351" t="b">
-        <f>(EXACT(A351,B351))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9606,7 +9607,7 @@
         <v>517</v>
       </c>
       <c r="H352" t="b">
-        <f>(EXACT(A352,B352))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9627,7 +9628,7 @@
         <v>542</v>
       </c>
       <c r="H353" t="b">
-        <f>(EXACT(A353,B353))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9648,7 +9649,7 @@
         <v>517</v>
       </c>
       <c r="H354" t="b">
-        <f>(EXACT(A354,B354))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9669,7 +9670,7 @@
         <v>503</v>
       </c>
       <c r="H355" t="b">
-        <f>(EXACT(A355,B355))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9690,7 +9691,7 @@
         <v>515</v>
       </c>
       <c r="H356" t="b">
-        <f>(EXACT(A356,B356))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9711,7 +9712,7 @@
         <v>477</v>
       </c>
       <c r="H357" t="b">
-        <f>(EXACT(A357,B357))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9732,7 +9733,7 @@
         <v>563</v>
       </c>
       <c r="H358" t="b">
-        <f>(EXACT(A358,B358))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9753,7 +9754,7 @@
         <v>542</v>
       </c>
       <c r="H359" t="b">
-        <f>(EXACT(A359,B359))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9774,7 +9775,7 @@
         <v>531</v>
       </c>
       <c r="H360" t="b">
-        <f>(EXACT(A360,B360))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9795,7 +9796,7 @@
         <v>542</v>
       </c>
       <c r="H361" t="b">
-        <f>(EXACT(A361,B361))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9816,7 +9817,7 @@
         <v>542</v>
       </c>
       <c r="H362" t="b">
-        <f>(EXACT(A362,B362))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9837,7 +9838,7 @@
         <v>563</v>
       </c>
       <c r="H363" t="b">
-        <f>(EXACT(A363,B363))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9858,7 +9859,7 @@
         <v>512</v>
       </c>
       <c r="H364" t="b">
-        <f>(EXACT(A364,B364))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9879,7 +9880,7 @@
         <v>492</v>
       </c>
       <c r="H365" t="b">
-        <f>(EXACT(A365,B365))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9900,7 +9901,7 @@
         <v>563</v>
       </c>
       <c r="H366" t="b">
-        <f>(EXACT(A366,B366))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9921,7 +9922,7 @@
         <v>542</v>
       </c>
       <c r="H367" t="b">
-        <f>(EXACT(A367,B367))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9942,7 +9943,7 @@
         <v>542</v>
       </c>
       <c r="H368" t="b">
-        <f>(EXACT(A368,B368))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9963,7 +9964,7 @@
         <v>542</v>
       </c>
       <c r="H369" t="b">
-        <f>(EXACT(A369,B369))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -9984,7 +9985,7 @@
         <v>506</v>
       </c>
       <c r="H370" t="b">
-        <f>(EXACT(A370,B370))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -10005,7 +10006,7 @@
         <v>544</v>
       </c>
       <c r="H371" t="b">
-        <f>(EXACT(A371,B371))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -10026,7 +10027,7 @@
         <v>572</v>
       </c>
       <c r="H372" t="b">
-        <f>(EXACT(A372,B372))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -10047,7 +10048,7 @@
         <v>542</v>
       </c>
       <c r="H373" t="b">
-        <f>(EXACT(A373,B373))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -10068,7 +10069,7 @@
         <v>479</v>
       </c>
       <c r="H374" t="b">
-        <f>(EXACT(A374,B374))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -10089,7 +10090,7 @@
         <v>487</v>
       </c>
       <c r="H375" t="b">
-        <f>(EXACT(A375,B375))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -10110,7 +10111,7 @@
         <v>559</v>
       </c>
       <c r="H376" t="b">
-        <f>(EXACT(A376,B376))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -10131,7 +10132,7 @@
         <v>517</v>
       </c>
       <c r="H377" t="b">
-        <f>(EXACT(A377,B377))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -10152,7 +10153,7 @@
         <v>542</v>
       </c>
       <c r="H378" t="b">
-        <f>(EXACT(A378,B378))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -10173,7 +10174,7 @@
         <v>505</v>
       </c>
       <c r="H379" t="b">
-        <f>(EXACT(A379,B379))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -10194,7 +10195,7 @@
         <v>523</v>
       </c>
       <c r="H380" t="b">
-        <f>(EXACT(A380,B380))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -10215,7 +10216,7 @@
         <v>515</v>
       </c>
       <c r="H381" t="b">
-        <f>(EXACT(A381,B381))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -10236,7 +10237,7 @@
         <v>542</v>
       </c>
       <c r="H382" t="b">
-        <f>(EXACT(A382,B382))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -10257,7 +10258,7 @@
         <v>480</v>
       </c>
       <c r="H383" t="b">
-        <f>(EXACT(A383,B383))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -10278,7 +10279,7 @@
         <v>534</v>
       </c>
       <c r="H384" t="b">
-        <f>(EXACT(A384,B384))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -10299,7 +10300,7 @@
         <v>480</v>
       </c>
       <c r="H385" t="b">
-        <f>(EXACT(A385,B385))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -10320,7 +10321,7 @@
         <v>480</v>
       </c>
       <c r="H386" t="b">
-        <f>(EXACT(A386,B386))</f>
+        <f t="shared" ref="H386:H449" si="6">(EXACT(A386,B386))</f>
         <v>1</v>
       </c>
     </row>
@@ -10341,7 +10342,7 @@
         <v>586</v>
       </c>
       <c r="H387" t="b">
-        <f>(EXACT(A387,B387))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10362,7 +10363,7 @@
         <v>517</v>
       </c>
       <c r="H388" t="b">
-        <f>(EXACT(A388,B388))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10383,7 +10384,7 @@
         <v>538</v>
       </c>
       <c r="H389" t="b">
-        <f>(EXACT(A389,B389))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10404,7 +10405,7 @@
         <v>580</v>
       </c>
       <c r="H390" t="b">
-        <f>(EXACT(A390,B390))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10425,7 +10426,7 @@
         <v>518</v>
       </c>
       <c r="H391" t="b">
-        <f>(EXACT(A391,B391))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10446,7 +10447,7 @@
         <v>500</v>
       </c>
       <c r="H392" t="b">
-        <f>(EXACT(A392,B392))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10467,7 +10468,7 @@
         <v>544</v>
       </c>
       <c r="H393" t="b">
-        <f>(EXACT(A393,B393))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10488,7 +10489,7 @@
         <v>544</v>
       </c>
       <c r="H394" t="b">
-        <f>(EXACT(A394,B394))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10509,7 +10510,7 @@
         <v>514</v>
       </c>
       <c r="H395" t="b">
-        <f>(EXACT(A395,B395))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10530,7 +10531,7 @@
         <v>483</v>
       </c>
       <c r="H396" t="b">
-        <f>(EXACT(A396,B396))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10551,7 +10552,7 @@
         <v>583</v>
       </c>
       <c r="H397" t="b">
-        <f>(EXACT(A397,B397))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10572,7 +10573,7 @@
         <v>477</v>
       </c>
       <c r="H398" t="b">
-        <f>(EXACT(A398,B398))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10593,7 +10594,7 @@
         <v>555</v>
       </c>
       <c r="H399" t="b">
-        <f>(EXACT(A399,B399))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10614,7 +10615,7 @@
         <v>542</v>
       </c>
       <c r="H400" t="b">
-        <f>(EXACT(A400,B400))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10635,7 +10636,7 @@
         <v>556</v>
       </c>
       <c r="H401" t="b">
-        <f>(EXACT(A401,B401))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10656,7 +10657,7 @@
         <v>570</v>
       </c>
       <c r="H402" t="b">
-        <f>(EXACT(A402,B402))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10677,7 +10678,7 @@
         <v>509</v>
       </c>
       <c r="H403" t="b">
-        <f>(EXACT(A403,B403))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10698,7 +10699,7 @@
         <v>566</v>
       </c>
       <c r="H404" t="b">
-        <f>(EXACT(A404,B404))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10719,7 +10720,7 @@
         <v>501</v>
       </c>
       <c r="H405" t="b">
-        <f>(EXACT(A405,B405))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10740,7 +10741,7 @@
         <v>502</v>
       </c>
       <c r="H406" t="b">
-        <f>(EXACT(A406,B406))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10761,7 +10762,7 @@
         <v>578</v>
       </c>
       <c r="H407" t="b">
-        <f>(EXACT(A407,B407))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10782,7 +10783,7 @@
         <v>509</v>
       </c>
       <c r="H408" t="b">
-        <f>(EXACT(A408,B408))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10803,7 +10804,7 @@
         <v>506</v>
       </c>
       <c r="H409" t="b">
-        <f>(EXACT(A409,B409))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10824,7 +10825,7 @@
         <v>495</v>
       </c>
       <c r="H410" t="b">
-        <f>(EXACT(A410,B410))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10845,7 +10846,7 @@
         <v>542</v>
       </c>
       <c r="H411" t="b">
-        <f>(EXACT(A411,B411))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10866,7 +10867,7 @@
         <v>525</v>
       </c>
       <c r="H412" t="b">
-        <f>(EXACT(A412,B412))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10887,7 +10888,7 @@
         <v>576</v>
       </c>
       <c r="H413" t="b">
-        <f>(EXACT(A413,B413))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10908,7 +10909,7 @@
         <v>487</v>
       </c>
       <c r="H414" t="b">
-        <f>(EXACT(A414,B414))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10929,7 +10930,7 @@
         <v>576</v>
       </c>
       <c r="H415" t="b">
-        <f>(EXACT(A415,B415))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10950,7 +10951,7 @@
         <v>501</v>
       </c>
       <c r="H416" t="b">
-        <f>(EXACT(A416,B416))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10971,7 +10972,7 @@
         <v>561</v>
       </c>
       <c r="H417" t="b">
-        <f>(EXACT(A417,B417))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -10992,7 +10993,7 @@
         <v>490</v>
       </c>
       <c r="H418" t="b">
-        <f>(EXACT(A418,B418))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11013,7 +11014,7 @@
         <v>542</v>
       </c>
       <c r="H419" t="b">
-        <f>(EXACT(A419,B419))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11034,7 +11035,7 @@
         <v>542</v>
       </c>
       <c r="H420" t="b">
-        <f>(EXACT(A420,B420))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11055,7 +11056,7 @@
         <v>542</v>
       </c>
       <c r="H421" t="b">
-        <f>(EXACT(A421,B421))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11076,7 +11077,7 @@
         <v>501</v>
       </c>
       <c r="H422" t="b">
-        <f>(EXACT(A422,B422))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11097,7 +11098,7 @@
         <v>576</v>
       </c>
       <c r="H423" t="b">
-        <f>(EXACT(A423,B423))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11118,7 +11119,7 @@
         <v>495</v>
       </c>
       <c r="H424" t="b">
-        <f>(EXACT(A424,B424))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11139,7 +11140,7 @@
         <v>530</v>
       </c>
       <c r="H425" t="b">
-        <f>(EXACT(A425,B425))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11160,7 +11161,7 @@
         <v>532</v>
       </c>
       <c r="H426" t="b">
-        <f>(EXACT(A426,B426))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11181,7 +11182,7 @@
         <v>542</v>
       </c>
       <c r="H427" t="b">
-        <f>(EXACT(A427,B427))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11202,7 +11203,7 @@
         <v>501</v>
       </c>
       <c r="H428" t="b">
-        <f>(EXACT(A428,B428))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11223,7 +11224,7 @@
         <v>539</v>
       </c>
       <c r="H429" t="b">
-        <f>(EXACT(A429,B429))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11244,7 +11245,7 @@
         <v>529</v>
       </c>
       <c r="H430" t="b">
-        <f>(EXACT(A430,B430))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11265,7 +11266,7 @@
         <v>591</v>
       </c>
       <c r="H431" t="b">
-        <f>(EXACT(A431,B431))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11286,7 +11287,7 @@
         <v>486</v>
       </c>
       <c r="H432" t="b">
-        <f>(EXACT(A432,B432))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11307,7 +11308,7 @@
         <v>541</v>
       </c>
       <c r="H433" t="b">
-        <f>(EXACT(A433,B433))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11328,7 +11329,7 @@
         <v>477</v>
       </c>
       <c r="H434" t="b">
-        <f>(EXACT(A434,B434))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11349,7 +11350,7 @@
         <v>493</v>
       </c>
       <c r="H435" t="b">
-        <f>(EXACT(A435,B435))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11370,7 +11371,7 @@
         <v>586</v>
       </c>
       <c r="H436" t="b">
-        <f>(EXACT(A436,B436))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11391,7 +11392,7 @@
         <v>497</v>
       </c>
       <c r="H437" t="b">
-        <f>(EXACT(A437,B437))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11412,7 +11413,7 @@
         <v>528</v>
       </c>
       <c r="H438" t="b">
-        <f>(EXACT(A438,B438))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11433,7 +11434,7 @@
         <v>526</v>
       </c>
       <c r="H439" t="b">
-        <f>(EXACT(A439,B439))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11454,7 +11455,7 @@
         <v>554</v>
       </c>
       <c r="H440" t="b">
-        <f>(EXACT(A440,B440))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11475,7 +11476,7 @@
         <v>545</v>
       </c>
       <c r="H441" t="b">
-        <f>(EXACT(A441,B441))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11496,7 +11497,7 @@
         <v>563</v>
       </c>
       <c r="H442" t="b">
-        <f>(EXACT(A442,B442))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11517,7 +11518,7 @@
         <v>515</v>
       </c>
       <c r="H443" t="b">
-        <f>(EXACT(A443,B443))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11538,7 +11539,7 @@
         <v>517</v>
       </c>
       <c r="H444" t="b">
-        <f>(EXACT(A444,B444))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11559,7 +11560,7 @@
         <v>517</v>
       </c>
       <c r="H445" t="b">
-        <f>(EXACT(A445,B445))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11580,7 +11581,7 @@
         <v>586</v>
       </c>
       <c r="H446" t="b">
-        <f>(EXACT(A446,B446))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11601,7 +11602,7 @@
         <v>542</v>
       </c>
       <c r="H447" t="b">
-        <f>(EXACT(A447,B447))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11622,7 +11623,7 @@
         <v>508</v>
       </c>
       <c r="H448" t="b">
-        <f>(EXACT(A448,B448))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11643,7 +11644,7 @@
         <v>515</v>
       </c>
       <c r="H449" t="b">
-        <f>(EXACT(A449,B449))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -11664,7 +11665,7 @@
         <v>542</v>
       </c>
       <c r="H450" t="b">
-        <f>(EXACT(A450,B450))</f>
+        <f t="shared" ref="H450:H468" si="7">(EXACT(A450,B450))</f>
         <v>1</v>
       </c>
     </row>
@@ -11685,7 +11686,7 @@
         <v>585</v>
       </c>
       <c r="H451" t="b">
-        <f>(EXACT(A451,B451))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -11706,7 +11707,7 @@
         <v>542</v>
       </c>
       <c r="H452" t="b">
-        <f>(EXACT(A452,B452))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -11727,7 +11728,7 @@
         <v>531</v>
       </c>
       <c r="H453" t="b">
-        <f>(EXACT(A453,B453))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -11748,7 +11749,7 @@
         <v>542</v>
       </c>
       <c r="H454" t="b">
-        <f>(EXACT(A454,B454))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -11769,7 +11770,7 @@
         <v>569</v>
       </c>
       <c r="H455" t="b">
-        <f>(EXACT(A455,B455))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -11790,7 +11791,7 @@
         <v>504</v>
       </c>
       <c r="H456" t="b">
-        <f>(EXACT(A456,B456))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -11811,7 +11812,7 @@
         <v>550</v>
       </c>
       <c r="H457" t="b">
-        <f>(EXACT(A457,B457))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -11832,7 +11833,7 @@
         <v>542</v>
       </c>
       <c r="H458" t="b">
-        <f>(EXACT(A458,B458))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -11853,7 +11854,7 @@
         <v>540</v>
       </c>
       <c r="H459" t="b">
-        <f>(EXACT(A459,B459))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -11874,7 +11875,7 @@
         <v>586</v>
       </c>
       <c r="H460" t="b">
-        <f>(EXACT(A460,B460))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -11895,7 +11896,7 @@
         <v>592</v>
       </c>
       <c r="H461" t="b">
-        <f>(EXACT(A461,B461))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -11916,7 +11917,7 @@
         <v>576</v>
       </c>
       <c r="H462" t="b">
-        <f>(EXACT(A462,B462))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -11937,7 +11938,7 @@
         <v>576</v>
       </c>
       <c r="H463" t="b">
-        <f>(EXACT(A463,B463))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -11958,7 +11959,7 @@
         <v>491</v>
       </c>
       <c r="H464" t="b">
-        <f>(EXACT(A464,B464))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -11979,7 +11980,7 @@
         <v>531</v>
       </c>
       <c r="H465" t="b">
-        <f>(EXACT(A465,B465))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -12000,7 +12001,7 @@
         <v>572</v>
       </c>
       <c r="H466" t="b">
-        <f>(EXACT(A466,B466))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -12021,7 +12022,7 @@
         <v>582</v>
       </c>
       <c r="H467" t="b">
-        <f>(EXACT(A467,B467))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -12042,7 +12043,7 @@
         <v>544</v>
       </c>
       <c r="H468" t="b">
-        <f>(EXACT(A468,B468))</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -12063,7 +12064,7 @@
         <v>567</v>
       </c>
       <c r="H469" t="b">
-        <f t="shared" ref="H469:H493" si="0">(EXACT(A469,B469))</f>
+        <f t="shared" ref="H469:H493" si="8">(EXACT(A469,B469))</f>
         <v>1</v>
       </c>
     </row>
@@ -12084,7 +12085,7 @@
         <v>544</v>
       </c>
       <c r="H470" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -12105,7 +12106,7 @@
         <v>505</v>
       </c>
       <c r="H471" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -12126,7 +12127,7 @@
         <v>544</v>
       </c>
       <c r="H472" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -12147,7 +12148,7 @@
         <v>529</v>
       </c>
       <c r="H473" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -12168,7 +12169,7 @@
         <v>522</v>
       </c>
       <c r="H474" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -12189,7 +12190,7 @@
         <v>542</v>
       </c>
       <c r="H475" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -12210,7 +12211,7 @@
         <v>503</v>
       </c>
       <c r="H476" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -12231,7 +12232,7 @@
         <v>526</v>
       </c>
       <c r="H477" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -12252,7 +12253,7 @@
         <v>542</v>
       </c>
       <c r="H478" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -12273,7 +12274,7 @@
         <v>512</v>
       </c>
       <c r="H479" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -12294,7 +12295,7 @@
         <v>544</v>
       </c>
       <c r="H480" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -12315,7 +12316,7 @@
         <v>544</v>
       </c>
       <c r="H481" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -12336,7 +12337,7 @@
         <v>567</v>
       </c>
       <c r="H482" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -12357,7 +12358,7 @@
         <v>526</v>
       </c>
       <c r="H483" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -12378,7 +12379,7 @@
         <v>529</v>
       </c>
       <c r="H484" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -12399,7 +12400,7 @@
         <v>508</v>
       </c>
       <c r="H485" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -12420,7 +12421,7 @@
         <v>535</v>
       </c>
       <c r="H486" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -12441,7 +12442,7 @@
         <v>500</v>
       </c>
       <c r="H487" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -12462,7 +12463,7 @@
         <v>499</v>
       </c>
       <c r="H488" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -12483,7 +12484,7 @@
         <v>515</v>
       </c>
       <c r="H489" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -12504,7 +12505,7 @@
         <v>576</v>
       </c>
       <c r="H490" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -12525,7 +12526,7 @@
         <v>532</v>
       </c>
       <c r="H491" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -12546,7 +12547,7 @@
         <v>542</v>
       </c>
       <c r="H492" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -12567,7 +12568,7 @@
         <v>542</v>
       </c>
       <c r="H493" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>